<commit_message>
Fix range in urls.py for loop
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -469,6 +469,114 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>3G SNC DI PAOLO GRANELLI &amp;amp; CO.</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>amministrazione@salsanatura.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>3G SNC DI PAOLO GRANELLI &amp;amp; CO.</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>amministrazione@salsanatura.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>A RICCHIGIA SRL</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>aricchigia@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>3G SNC DI PAOLO GRANELLI &amp;amp; CO.</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>amministrazione@salsanatura.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>A RICCHIGIA SRL</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>aricchigia@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>A. DARBO AG</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>katrin.widauer@darbo.at</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>A. GANDOLA &amp;amp; C. SPA</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>gandola@gandola.it</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>A. GANDOLA &amp;amp; C. SPA</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>gandola@gandola.it</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>A. LOACKER SPA</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>marketing@loacker.com</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Add logic to save nfc1 dictionary to nfc1.txt in emails.py
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -484,96 +484,180 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>3G SNC DI PAOLO GRANELLI &amp;amp; CO.</t>
+          <t>A RICCHIGIA SRL</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>amministrazione@salsanatura.com</t>
+          <t>aricchigia@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>A RICCHIGIA SRL</t>
+          <t>A. DARBO AG</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>aricchigia@gmail.com</t>
+          <t>katrin.widauer@darbo.at</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>3G SNC DI PAOLO GRANELLI &amp;amp; CO.</t>
+          <t>A. GANDOLA &amp;amp; C. SPA</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>amministrazione@salsanatura.com</t>
+          <t>gandola@gandola.it</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>A RICCHIGIA SRL</t>
+          <t>A. LOACKER SPA</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>aricchigia@gmail.com</t>
+          <t>marketing@loacker.com</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>A. DARBO AG</t>
+          <t>A.D. SRL</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>katrin.widauer@darbo.at</t>
+          <t>info@aiellobio.it</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>A. GANDOLA &amp;amp; C. SPA</t>
+          <t>A.O.C. SOCIETA' COOP. AGRICOLA</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>gandola@gandola.it</t>
+          <t>info@calabriaaoc.it</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>A. GANDOLA &amp;amp; C. SPA</t>
+          <t>A.R. TARTUFI SRL</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>gandola@gandola.it</t>
+          <t>commerciale@valnerinatartufi.com</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>A. LOACKER SPA</t>
+          <t>AB MAURI ITALY SPA</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>marketing@loacker.com</t>
+          <t>italy.accounting@abmauri.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>ACCADEMIA DEL PANE</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Not found/case 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>ACCADEMIA GROUP SRL</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>redazione@ristorazioneitalianamagazine.it</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>ACCADEMIA OLEARIA SRL</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>commerciale@accademiaolearia.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>ACCUDIRE SRL</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>info@accudire.eu</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>ACEITUNAS SANMER OLIVES</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>INFO@SANMER.COM</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>ACEITUNAS TORREMAR</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Not found/case 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>ACETAIA BORGO CASTELLO SRL</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>avivici@acetaiaborgocastello.it</t>
         </is>
       </c>
     </row>

</xml_diff>